<commit_message>
Se agrega descripción a ficha tecnica, fix views
</commit_message>
<xml_diff>
--- a/storage/app/public/ficha_tecnica_subdivision.xlsx
+++ b/storage/app/public/ficha_tecnica_subdivision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ODS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F809C-1834-4E64-871C-0462636C967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD95A8F-1A6A-4368-8AC0-F8019DC63FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59A6636E-DD9B-4BB2-A6F8-8B43A0BBD60A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59A6636E-DD9B-4BB2-A6F8-8B43A0BBD60A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="163">
   <si>
     <t>Cuenta Predial</t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>divisa_gravamen</t>
+  </si>
+  <si>
+    <t>descripcion</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -635,6 +638,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -647,7 +654,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,133 +968,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE6CF71-2ADA-45B0-88E2-9CF8220A3B5B}">
-  <dimension ref="A1:BB14"/>
+  <dimension ref="A1:BC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3:AY1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.33203125" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.21875" customWidth="1"/>
-    <col min="29" max="29" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="49.21875" customWidth="1"/>
-    <col min="47" max="47" width="24" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.6640625" customWidth="1"/>
-    <col min="50" max="50" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25.77734375" style="10" customWidth="1"/>
-    <col min="52" max="52" width="35.88671875" customWidth="1"/>
-    <col min="53" max="53" width="36.21875" customWidth="1"/>
-    <col min="54" max="54" width="44.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43" style="1" customWidth="1"/>
+    <col min="20" max="20" width="35.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.28515625" customWidth="1"/>
+    <col min="30" max="30" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="49.28515625" customWidth="1"/>
+    <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" customWidth="1"/>
+    <col min="51" max="51" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="25.7109375" style="7" customWidth="1"/>
+    <col min="53" max="53" width="35.85546875" customWidth="1"/>
+    <col min="54" max="54" width="36.28515625" customWidth="1"/>
+    <col min="55" max="55" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="3" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="4" t="s">
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1144,124 +1152,127 @@
         <v>18</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BC2" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="BA8" s="5"/>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BB8" s="5"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="G14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="T1:AS1"/>
-    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="U1:AT1"/>
+    <mergeCell ref="AV1:BC1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:R1"/>
   </mergeCells>
@@ -1280,31 +1291,31 @@
           <x14:formula1>
             <xm:f>Hoja2!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Q3:Q1048576 AX3:AX1048576</xm:sqref>
+          <xm:sqref>Q3:Q1048576 AY3:AY1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{97037693-4E07-4C50-A193-BB1B6FD2E397}">
           <x14:formula1>
             <xm:f>Hoja2!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R3:R1048576</xm:sqref>
+          <xm:sqref>R3:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A829656-F05A-470D-8E21-3E3C07FCDC23}">
           <x14:formula1>
             <xm:f>Hoja2!$D$2:$D$31</xm:f>
           </x14:formula1>
-          <xm:sqref>T3:T1048576</xm:sqref>
+          <xm:sqref>U3:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D628FB9B-B223-42FC-9212-4C6E83F673BA}">
           <x14:formula1>
             <xm:f>Hoja2!$E$2:$E$45</xm:f>
           </x14:formula1>
-          <xm:sqref>U3:U1048576</xm:sqref>
+          <xm:sqref>V3:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CFF5AEEF-3A0F-42CD-AE52-DCA6A339BCCE}">
           <x14:formula1>
             <xm:f>Hoja2!$H$2:$H$17</xm:f>
           </x14:formula1>
-          <xm:sqref>AU3:AU1048576</xm:sqref>
+          <xm:sqref>AV3:AV1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1320,15 +1331,15 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1354,7 +1365,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1380,7 +1391,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1406,7 +1417,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>67</v>
       </c>
@@ -1443,7 +1454,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>68</v>
       </c>
@@ -1460,7 +1471,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>69</v>
       </c>
@@ -1477,7 +1488,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>70</v>
       </c>
@@ -1491,7 +1502,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>71</v>
       </c>
@@ -1505,7 +1516,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>72</v>
       </c>
@@ -1519,7 +1530,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>73</v>
       </c>
@@ -1533,7 +1544,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>74</v>
       </c>
@@ -1547,7 +1558,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>75</v>
       </c>
@@ -1561,7 +1572,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>76</v>
       </c>
@@ -1575,7 +1586,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>77</v>
       </c>
@@ -1589,7 +1600,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>78</v>
       </c>
@@ -1603,7 +1614,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>79</v>
       </c>
@@ -1617,7 +1628,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>80</v>
       </c>
@@ -1628,7 +1639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>81</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>82</v>
       </c>
@@ -1650,7 +1661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>83</v>
       </c>
@@ -1658,7 +1669,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>84</v>
       </c>
@@ -1666,7 +1677,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>85</v>
       </c>
@@ -1674,7 +1685,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>86</v>
       </c>
@@ -1682,7 +1693,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>87</v>
       </c>
@@ -1690,7 +1701,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>88</v>
       </c>
@@ -1698,7 +1709,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>89</v>
       </c>
@@ -1706,7 +1717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>90</v>
       </c>
@@ -1714,7 +1725,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>91</v>
       </c>
@@ -1722,7 +1733,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>92</v>
       </c>
@@ -1730,7 +1741,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>93</v>
       </c>
@@ -1738,72 +1749,72 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>134</v>
       </c>

</xml_diff>